<commit_message>
Salary NA's and beginning of Outlier section
</commit_message>
<xml_diff>
--- a/Masters Project Fall Placement/Data dictionary.xlsx
+++ b/Masters Project Fall Placement/Data dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yawel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Hondrakis\OneDrive\Documents\DataAnalysis\Masters Project Fall Placement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EC6A9F3-19FB-4975-8C21-809692A49399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D2A3F6-B16E-49CB-827F-D7E65C1F3D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" xr2:uid="{EBE4050F-CE21-4014-9885-B02367D8F75B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EBE4050F-CE21-4014-9885-B02367D8F75B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,13 +125,13 @@
     <t>status</t>
   </si>
   <si>
-    <t>placed or nor placed (target variable)</t>
-  </si>
-  <si>
     <t>Secondary Education percentile</t>
   </si>
   <si>
     <t>Employability test percentile</t>
+  </si>
+  <si>
+    <t>placed or not placed (target variable)</t>
   </si>
 </sst>
 </file>
@@ -495,16 +495,16 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -512,7 +512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -520,7 +520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -528,15 +528,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -544,7 +544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -552,7 +552,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -560,7 +560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -568,7 +568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -576,7 +576,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -584,7 +584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -592,15 +592,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -608,7 +608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -616,7 +616,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -624,12 +624,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>